<commit_message>
fixed validation formula in sample submission template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v0.14.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v0.14.xlsx
@@ -1675,7 +1675,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
@@ -1830,7 +1830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>3</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>4</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>5</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>6</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>7</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>8</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>9</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>10</v>
       </c>
@@ -2110,7 +2110,7 @@
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>11</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>12</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>13</v>
       </c>
@@ -17481,7 +17481,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
-      <formula1>IF(OR(#REF!="Tube",#REF!="96-well plate"),Index!$A$2:$A$97,IF(#REF!="384-well plate",Index!$B$2:$B$385,""))</formula1>
+      <formula1>IF(OR($H8="Tube",$H8="96-well plate"),Index!$A$2:$A$97,IF($H8="384-well plate",Index!$B$2:$B$385,""))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -17507,7 +17507,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.38"/>

</xml_diff>

<commit_message>
Propagating change done on qc. Fix sample submission validation on coord column.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v0.14.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v0.14.xlsx
@@ -1675,7 +1675,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
@@ -1830,7 +1830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>3</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>4</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>5</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>6</v>
       </c>
@@ -1998,7 +1998,7 @@
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>7</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>8</v>
       </c>
@@ -2054,7 +2054,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>9</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>10</v>
       </c>
@@ -2110,7 +2110,7 @@
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>11</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>12</v>
       </c>
@@ -2166,7 +2166,7 @@
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>13</v>
       </c>
@@ -17481,7 +17481,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
-      <formula1>IF(OR(#REF!="Tube",#REF!="96-well plate"),Index!$A$2:$A$97,IF(#REF!="384-well plate",Index!$B$2:$B$385,""))</formula1>
+      <formula1>IF(OR($H8="Tube",$H8="96-well plate"),Index!$A$2:$A$97,IF($H8="384-well plate",Index!$B$2:$B$385,""))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -17507,7 +17507,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.38"/>

</xml_diff>